<commit_message>
Technical change & Update wiki
</commit_message>
<xml_diff>
--- a/tables/sample_data.xlsx
+++ b/tables/sample_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bm\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bm\Desktop\Developing-Variety-Of-Methods-For-Identifying-Anomalies-\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811B96CB-D07E-4E1E-9D6B-1E5F1E450414}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1993F51E-4DB9-4252-95C0-F07CFE5AAF97}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4485" xr2:uid="{E303D615-DEF1-4AEB-BA46-C7DB623A6C3F}"/>
   </bookViews>
@@ -511,7 +511,7 @@
   <dimension ref="A1:AM120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:AL1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>